<commit_message>
update project files and ignore node_modules, dist
</commit_message>
<xml_diff>
--- a/public/data/arz_mabar.xlsx
+++ b/public/data/arz_mabar.xlsx
@@ -1,56 +1,61 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr dateCompatibility="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kowsar\Desktop\محلات\mahalle-artesh\public\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kowsar\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F2305F6F-F4BD-4820-8E9A-02BF2838D644}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100008_{D0109CF2-081D-4AA4-8119-B3A3B7BDFE66}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9090" xr2:uid="{7A3952D8-9A7C-4AB1-B441-E6D13B8267DF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="5985" xr2:uid="{814F4C6E-3F6A-4179-9920-24703E9B594F}"/>
   </bookViews>
   <sheets>
-    <sheet name="arz_mabar_m14" sheetId="1" r:id="rId1"/>
+    <sheet name="arz_mabaar" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="2" uniqueCount="2">
+  <si>
+    <t>عرض معبر</t>
+  </si>
   <si>
     <t>تعداد</t>
-  </si>
-  <si>
-    <t>عرض معبر</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="Aptos Display"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -58,7 +63,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -66,7 +71,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -74,35 +79,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -110,7 +115,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -118,14 +123,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -133,14 +138,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -148,7 +153,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -156,19 +161,19 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -346,26 +351,20 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="10">
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom style="thick">
         <color theme="4"/>
@@ -373,8 +372,8 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom style="thick">
         <color theme="4" tint="0.499984740745262"/>
@@ -382,8 +381,8 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.39997558519241921"/>
@@ -391,12 +390,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <start style="thin">
         <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
+      </start>
+      <end style="thin">
         <color rgb="FF7F7F7F"/>
-      </right>
+      </end>
       <top style="thin">
         <color rgb="FF7F7F7F"/>
       </top>
@@ -406,12 +405,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <start style="thin">
         <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
+      </start>
+      <end style="thin">
         <color rgb="FF3F3F3F"/>
-      </right>
+      </end>
       <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
@@ -421,8 +420,8 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -430,12 +429,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <start style="double">
         <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
+      </start>
+      <end style="double">
         <color rgb="FF3F3F3F"/>
-      </right>
+      </end>
       <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
@@ -445,12 +444,12 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <start style="thin">
         <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
+      </start>
+      <end style="thin">
         <color rgb="FFB2B2B2"/>
-      </right>
+      </end>
       <top style="thin">
         <color rgb="FFB2B2B2"/>
       </top>
@@ -460,8 +459,8 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -515,9 +514,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -577,7 +575,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -587,39 +585,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -671,7 +669,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -730,25 +728,25 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:lumMod val="110%"/>
+                <a:satMod val="105%"/>
+                <a:tint val="67%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:lumMod val="105%"/>
+                <a:satMod val="103%"/>
+                <a:tint val="73%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:lumMod val="105%"/>
+                <a:satMod val="109%"/>
+                <a:tint val="81%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -756,25 +754,25 @@
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:satMod val="103%"/>
+                <a:lumMod val="102%"/>
+                <a:tint val="94%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:satMod val="110%"/>
+                <a:lumMod val="100%"/>
+                <a:shade val="100%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:lumMod val="99%"/>
+                <a:satMod val="120%"/>
+                <a:shade val="78%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -782,26 +780,26 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800%"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -815,7 +813,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="63%"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -827,32 +825,32 @@
         </a:solidFill>
         <a:solidFill>
           <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
+            <a:tint val="95%"/>
+            <a:satMod val="170%"/>
           </a:schemeClr>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="93%"/>
+                <a:satMod val="150%"/>
+                <a:shade val="98%"/>
+                <a:lumMod val="102%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="98%"/>
+                <a:satMod val="130%"/>
+                <a:shade val="90%"/>
+                <a:lumMod val="103%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="63%"/>
+                <a:satMod val="120%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -861,35 +859,55 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F28F0A-C78A-4929-ACCE-45A024EB3C28}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAA20089-7A1E-4781-854F-E9DF7BFC3E3A}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A2" sqref="A2:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>6</v>
       </c>
@@ -897,7 +915,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>8</v>
       </c>
@@ -905,7 +923,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>10</v>
       </c>
@@ -913,7 +931,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5">
         <v>16</v>
       </c>
@@ -921,7 +939,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6">
         <v>18</v>
       </c>
@@ -929,7 +947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7">
         <v>20</v>
       </c>
@@ -937,7 +955,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8">
         <v>24</v>
       </c>
@@ -945,7 +963,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9">
         <v>30</v>
       </c>
@@ -953,7 +971,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10">
         <v>32</v>
       </c>
@@ -963,6 +981,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>